<commit_message>
added median salaries for data science and graphic design
</commit_message>
<xml_diff>
--- a/data/Moto_Industry_Companies.xlsx
+++ b/data/Moto_Industry_Companies.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="144">
   <si>
     <t>Company_Name</t>
   </si>
@@ -60,105 +60,202 @@
     <t>avg_cost_transportation</t>
   </si>
   <si>
+    <t>median_salary_graphic_designer_senior</t>
+  </si>
+  <si>
+    <t>median_salary_data_scienitst_entry</t>
+  </si>
+  <si>
+    <t>REV'IT! Sport USA</t>
+  </si>
+  <si>
+    <t>275 Conover Street 5P</t>
+  </si>
+  <si>
+    <t>NY</t>
+  </si>
+  <si>
+    <t>Gear</t>
+  </si>
+  <si>
+    <t>Brooklyn</t>
+  </si>
+  <si>
+    <t>RevZilla</t>
+  </si>
+  <si>
+    <t>4020 S. 26th Street</t>
+  </si>
+  <si>
+    <t>PA</t>
+  </si>
+  <si>
+    <t>Website</t>
+  </si>
+  <si>
+    <t>Philadelphia</t>
+  </si>
+  <si>
+    <t>Triumph Motorcycles America</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100 Hartsfield Center Pkwy #200 </t>
+  </si>
+  <si>
+    <t>GA</t>
+  </si>
+  <si>
+    <t>Manufacture</t>
+  </si>
+  <si>
+    <t>Atlanta</t>
+  </si>
+  <si>
+    <t>CycleLogic Inc. Engine Ice</t>
+  </si>
+  <si>
+    <t>125 E Merritt Island Causeway
+Suite 107-401</t>
+  </si>
+  <si>
+    <t>FL</t>
+  </si>
+  <si>
+    <t>Fluids</t>
+  </si>
+  <si>
+    <t>Merritt Island</t>
+  </si>
+  <si>
+    <t>Cardo Systems, Inc.</t>
+  </si>
+  <si>
+    <t>811 E Plano Pkwy #110a</t>
+  </si>
+  <si>
+    <t>TX</t>
+  </si>
+  <si>
+    <t>Tech</t>
+  </si>
+  <si>
+    <t>Plano</t>
+  </si>
+  <si>
+    <t>Klim USA</t>
+  </si>
+  <si>
+    <t>3753 E County Line Rd</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Rigby</t>
+  </si>
+  <si>
+    <t>Ruroc</t>
+  </si>
+  <si>
+    <t>UT</t>
+  </si>
+  <si>
+    <t>Helmets</t>
+  </si>
+  <si>
+    <t>Ogden</t>
+  </si>
+  <si>
+    <t>Rockstar Energy Drink</t>
+  </si>
+  <si>
+    <t>CA</t>
+  </si>
+  <si>
+    <t>Energy Drink</t>
+  </si>
+  <si>
+    <t>Los Angeles</t>
+  </si>
+  <si>
+    <t>Red Bull Media House</t>
+  </si>
+  <si>
+    <t>Manhattan Beach</t>
+  </si>
+  <si>
+    <t>Red Bull North America</t>
+  </si>
+  <si>
+    <t>2700 Pennsylvania Ave #1100</t>
+  </si>
+  <si>
+    <t>Santa Monica</t>
+  </si>
+  <si>
+    <t>International Motorcycle Shows</t>
+  </si>
+  <si>
+    <t>2901 28th St, Ste. 100</t>
+  </si>
+  <si>
+    <t>Show</t>
+  </si>
+  <si>
+    <t>Alpinestars</t>
+  </si>
+  <si>
+    <t>2780 W 237th St</t>
+  </si>
+  <si>
+    <t>Torrance</t>
+  </si>
+  <si>
+    <t>Yamaha Motor Corp.</t>
+  </si>
+  <si>
+    <t>6555 Katella Ave</t>
+  </si>
+  <si>
+    <t>Cypress</t>
+  </si>
+  <si>
+    <t>HJC America, Inc.</t>
+  </si>
+  <si>
+    <t>511 S Harbor Blvd STE V</t>
+  </si>
+  <si>
+    <t>La Habra</t>
+  </si>
+  <si>
+    <t>Scorpion Sports, Inc.</t>
+  </si>
+  <si>
+    <t>12145 Mora Dr #13</t>
+  </si>
+  <si>
+    <t>Santa Fe Springs</t>
+  </si>
+  <si>
+    <t>Vance &amp; Hines</t>
+  </si>
+  <si>
+    <t>13861 Rosecrans Ave</t>
+  </si>
+  <si>
+    <t>Aftermarket</t>
+  </si>
+  <si>
     <t>Spidi Inc.</t>
   </si>
   <si>
     <t>29229 Canwood St, STE 202</t>
   </si>
   <si>
-    <t>CA</t>
-  </si>
-  <si>
-    <t>Gear</t>
-  </si>
-  <si>
     <t>Agoura Hills</t>
   </si>
   <si>
-    <t>Schuberth North America</t>
-  </si>
-  <si>
-    <t>33 Journey Suite 200</t>
-  </si>
-  <si>
-    <t>Helmets</t>
-  </si>
-  <si>
-    <t>Aliso Viejo</t>
-  </si>
-  <si>
-    <t>Kendon Industries, LLC</t>
-  </si>
-  <si>
-    <t>2990 E. Miraloma Ave.</t>
-  </si>
-  <si>
-    <t>Trailers</t>
-  </si>
-  <si>
-    <t>Anaheim</t>
-  </si>
-  <si>
-    <t>Triumph Motorcycles America</t>
-  </si>
-  <si>
-    <t xml:space="preserve">100 Hartsfield Center Pkwy #200 </t>
-  </si>
-  <si>
-    <t>GA</t>
-  </si>
-  <si>
-    <t>Manufacture</t>
-  </si>
-  <si>
-    <t>Atlanta</t>
-  </si>
-  <si>
-    <t>Kreft Moto</t>
-  </si>
-  <si>
-    <t>20780 High Desert Lane</t>
-  </si>
-  <si>
-    <t>OR</t>
-  </si>
-  <si>
-    <t>Aftermarket</t>
-  </si>
-  <si>
-    <t>Bend</t>
-  </si>
-  <si>
-    <t>Cycle Gear</t>
-  </si>
-  <si>
-    <t>4705 Industrial Way</t>
-  </si>
-  <si>
-    <t>Benicia</t>
-  </si>
-  <si>
-    <t>Suzuki Motor of America, Inc.</t>
-  </si>
-  <si>
-    <t>P.O. BOX 1100</t>
-  </si>
-  <si>
-    <t>Brea</t>
-  </si>
-  <si>
-    <t>REV'IT! Sport USA</t>
-  </si>
-  <si>
-    <t>275 Conover Street 5P</t>
-  </si>
-  <si>
-    <t>NY</t>
-  </si>
-  <si>
-    <t>Brooklyn</t>
-  </si>
-  <si>
     <t>Yoshimura R&amp;D of America, Inc.</t>
   </si>
   <si>
@@ -168,67 +265,16 @@
     <t>Chino</t>
   </si>
   <si>
-    <t>Two Brothers Racing</t>
-  </si>
-  <si>
-    <t>167 Via Trevizio</t>
-  </si>
-  <si>
-    <t>Corona</t>
-  </si>
-  <si>
-    <t>Dainese USA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1645 Superior Ave </t>
-  </si>
-  <si>
-    <t>Costa Mesa</t>
-  </si>
-  <si>
-    <t>Ducati North America, Inc.</t>
-  </si>
-  <si>
-    <t>10443 Bandley Drive</t>
-  </si>
-  <si>
-    <t>Cupertino</t>
-  </si>
-  <si>
-    <t>Yamaha Motor Corp.</t>
-  </si>
-  <si>
-    <t>6555 Katella Ave</t>
-  </si>
-  <si>
-    <t>Cypress</t>
-  </si>
-  <si>
-    <t>Kawasaki Motor Corp.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">26972 Burbank </t>
-  </si>
-  <si>
-    <t>Foothill Ranch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fox Racing </t>
-  </si>
-  <si>
-    <t>16752 Armstrong Ave</t>
-  </si>
-  <si>
-    <t>Irvine</t>
-  </si>
-  <si>
-    <t>Sena Technologies, Inc.</t>
-  </si>
-  <si>
-    <t>152 Technology Dr.</t>
-  </si>
-  <si>
-    <t>Tech</t>
+    <t>Mountain Motorsports</t>
+  </si>
+  <si>
+    <t>1025 N. Mountain Ave</t>
+  </si>
+  <si>
+    <t>Dealership</t>
+  </si>
+  <si>
+    <t>Ontario</t>
   </si>
   <si>
     <r>
@@ -246,44 +292,16 @@
     <t>13960 Campo Rd</t>
   </si>
   <si>
-    <t>Website</t>
-  </si>
-  <si>
     <t>Jamul</t>
   </si>
   <si>
-    <t>HJC America, Inc.</t>
-  </si>
-  <si>
-    <t>511 S Harbor Blvd STE V</t>
-  </si>
-  <si>
-    <t>La Habra</t>
-  </si>
-  <si>
-    <t>Rockstar Energy Drink</t>
-  </si>
-  <si>
-    <t>Energy Drink</t>
-  </si>
-  <si>
-    <t>Los Angeles</t>
-  </si>
-  <si>
-    <t>CycleLogic Inc. Engine Ice</t>
-  </si>
-  <si>
-    <t>125 E Merritt Island Causeway
-Suite 107-401</t>
-  </si>
-  <si>
-    <t>FL</t>
-  </si>
-  <si>
-    <t>Fluids</t>
-  </si>
-  <si>
-    <t>Merritt Island</t>
+    <t>Maxima Racing Oils</t>
+  </si>
+  <si>
+    <t>4266 Abraham Way</t>
+  </si>
+  <si>
+    <t>Santee</t>
   </si>
   <si>
     <t>KTM North America, Inc.</t>
@@ -295,49 +313,118 @@
     <t>Murrieta</t>
   </si>
   <si>
-    <t>Ruroc</t>
-  </si>
-  <si>
-    <t>UT</t>
-  </si>
-  <si>
-    <t>Ogden</t>
-  </si>
-  <si>
-    <t>Mountain Motorsports</t>
-  </si>
-  <si>
-    <t>1025 N. Mountain Ave</t>
-  </si>
-  <si>
-    <t>Dealership</t>
-  </si>
-  <si>
-    <t>Ontario</t>
-  </si>
-  <si>
-    <t>RevZilla</t>
-  </si>
-  <si>
-    <t>4020 S. 26th Street</t>
-  </si>
-  <si>
-    <t>PA</t>
-  </si>
-  <si>
-    <t>Philadelphia</t>
-  </si>
-  <si>
-    <t>Cardo Systems, Inc.</t>
-  </si>
-  <si>
-    <t>811 E Plano Pkwy #110a</t>
-  </si>
-  <si>
-    <t>TX</t>
-  </si>
-  <si>
-    <t>Plano</t>
+    <t xml:space="preserve">Fox Racing </t>
+  </si>
+  <si>
+    <t>16752 Armstrong Ave</t>
+  </si>
+  <si>
+    <t>Irvine</t>
+  </si>
+  <si>
+    <t>Kawasaki Motor Corp.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26972 Burbank </t>
+  </si>
+  <si>
+    <t>Foothill Ranch</t>
+  </si>
+  <si>
+    <t>Sena Technologies, Inc.</t>
+  </si>
+  <si>
+    <t>152 Technology Dr.</t>
+  </si>
+  <si>
+    <t>Dainese USA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1645 Superior Ave </t>
+  </si>
+  <si>
+    <t>Costa Mesa</t>
+  </si>
+  <si>
+    <t>Schuberth North America</t>
+  </si>
+  <si>
+    <t>33 Journey Suite 200</t>
+  </si>
+  <si>
+    <t>Aliso Viejo</t>
+  </si>
+  <si>
+    <t>Kendon Industries, LLC</t>
+  </si>
+  <si>
+    <t>2990 E. Miraloma Ave.</t>
+  </si>
+  <si>
+    <t>Trailers</t>
+  </si>
+  <si>
+    <t>Anaheim</t>
+  </si>
+  <si>
+    <t>Suzuki Motor of America, Inc.</t>
+  </si>
+  <si>
+    <t>P.O. BOX 1100</t>
+  </si>
+  <si>
+    <t>Brea</t>
+  </si>
+  <si>
+    <t>Two Brothers Racing</t>
+  </si>
+  <si>
+    <t>167 Via Trevizio</t>
+  </si>
+  <si>
+    <t>Corona</t>
+  </si>
+  <si>
+    <t>GoPro</t>
+  </si>
+  <si>
+    <t>3025 Clearview Way</t>
+  </si>
+  <si>
+    <t>San Mateo</t>
+  </si>
+  <si>
+    <t>Cycle Gear</t>
+  </si>
+  <si>
+    <t>4705 Industrial Way</t>
+  </si>
+  <si>
+    <t>Benicia</t>
+  </si>
+  <si>
+    <t>Ducati North America, Inc.</t>
+  </si>
+  <si>
+    <t>10443 Bandley Drive</t>
+  </si>
+  <si>
+    <t>Cupertino</t>
+  </si>
+  <si>
+    <t>Bell Sports, Inc.</t>
+  </si>
+  <si>
+    <t>5550 Scotts Valley Dr</t>
+  </si>
+  <si>
+    <t>Scotts Valley</t>
+  </si>
+  <si>
+    <t>Fox Factory, Inc.</t>
+  </si>
+  <si>
+    <t>915 Disc Dr</t>
   </si>
   <si>
     <t>Icon Motosports</t>
@@ -346,6 +433,9 @@
     <t>1745 NW Marshall St</t>
   </si>
   <si>
+    <t>OR</t>
+  </si>
+  <si>
     <t>Portland</t>
   </si>
   <si>
@@ -355,97 +445,13 @@
     <t>15353 SW Sequoia Pkwy</t>
   </si>
   <si>
-    <t>Klim USA</t>
-  </si>
-  <si>
-    <t>3753 E County Line Rd</t>
-  </si>
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>Rigby</t>
-  </si>
-  <si>
-    <t>GoPro</t>
-  </si>
-  <si>
-    <t>3025 Clearview Way</t>
-  </si>
-  <si>
-    <t>San Mateo</t>
-  </si>
-  <si>
-    <t>Scorpion Sports, Inc.</t>
-  </si>
-  <si>
-    <t>12145 Mora Dr #13</t>
-  </si>
-  <si>
-    <t>Santa Fe Springs</t>
-  </si>
-  <si>
-    <t>Vance &amp; Hines</t>
-  </si>
-  <si>
-    <t>13861 Rosecrans Ave</t>
-  </si>
-  <si>
-    <t>Red Bull North America</t>
-  </si>
-  <si>
-    <t>2700 Pennsylvania Ave #1100</t>
-  </si>
-  <si>
-    <t>Santa Monica</t>
-  </si>
-  <si>
-    <t>International Motorcycle Shows</t>
-  </si>
-  <si>
-    <t>2901 28th St, Ste. 100</t>
-  </si>
-  <si>
-    <t>Show</t>
-  </si>
-  <si>
-    <t>Maxima Racing Oils</t>
-  </si>
-  <si>
-    <t>4266 Abraham Way</t>
-  </si>
-  <si>
-    <t>Santee</t>
-  </si>
-  <si>
-    <t>Bell Sports, Inc.</t>
-  </si>
-  <si>
-    <t>5550 Scotts Valley Dr</t>
-  </si>
-  <si>
-    <t>Scotts Valley</t>
-  </si>
-  <si>
-    <t>Fox Factory, Inc.</t>
-  </si>
-  <si>
-    <t>915 Disc Dr</t>
-  </si>
-  <si>
-    <t>Alpinestars</t>
-  </si>
-  <si>
-    <t>2780 W 237th St</t>
-  </si>
-  <si>
-    <t>Torrance</t>
-  </si>
-  <si>
-    <t>Red Bull Media House</t>
-  </si>
-  <si>
-    <t>Manhattan Beach</t>
+    <t>Kreft Moto</t>
+  </si>
+  <si>
+    <t>20780 High Desert Lane</t>
+  </si>
+  <si>
+    <t>Bend</t>
   </si>
   <si>
     <t>https://www.bestplaces.net/cost_of_living/city/california/agoura_hills</t>
@@ -455,7 +461,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -464,6 +470,11 @@
     <font>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font/>
+    <font>
+      <color rgb="FF000000"/>
+      <name val="Roboto"/>
     </font>
     <font>
       <u/>
@@ -478,12 +489,18 @@
       <color rgb="FF0000FF"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -492,7 +509,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -502,10 +519,16 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -778,589 +801,659 @@
       <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="P1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="3"/>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D2" s="1">
-        <v>91301.0</v>
+        <v>11231.0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="1">
-        <v>430.0</v>
+        <v>20</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="2">
+        <v>716.0</v>
       </c>
       <c r="H2" s="1">
-        <v>2534.0</v>
+        <v>2951.0</v>
       </c>
       <c r="I2" s="1">
-        <v>1027.0</v>
+        <v>651.0</v>
       </c>
       <c r="J2" s="1">
-        <v>20736.0</v>
+        <v>2635121.0</v>
       </c>
       <c r="K2" s="1">
         <v>4.2</v>
       </c>
       <c r="L2" s="1">
-        <v>44.0</v>
+        <v>34.8</v>
       </c>
       <c r="M2" s="1">
-        <v>105.3</v>
+        <v>117.78</v>
       </c>
       <c r="N2" s="1">
-        <v>97.3</v>
+        <v>151.16</v>
       </c>
       <c r="O2" s="1">
-        <v>158.5</v>
+        <v>192.6</v>
+      </c>
+      <c r="P2" s="1">
+        <v>92202.0</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>81391.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D3" s="1">
-        <v>92656.0</v>
+        <v>19112.0</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="G3" s="1">
-        <v>426.0</v>
+        <v>180.0</v>
       </c>
       <c r="H3" s="1">
-        <v>2248.0</v>
+        <v>1652.0</v>
       </c>
       <c r="I3" s="1">
-        <v>996.0</v>
+        <v>805.0</v>
       </c>
       <c r="J3" s="1">
-        <v>50691.0</v>
+        <v>1569657.0</v>
       </c>
       <c r="K3" s="1">
-        <v>2.6</v>
+        <v>5.6</v>
       </c>
       <c r="L3" s="1">
-        <v>36.6</v>
+        <v>34.1</v>
       </c>
       <c r="M3" s="1">
-        <v>102.7</v>
+        <v>102.5</v>
       </c>
       <c r="N3" s="1">
-        <v>101.5</v>
+        <v>107.7</v>
       </c>
       <c r="O3" s="1">
-        <v>111.3</v>
+        <v>141.9</v>
+      </c>
+      <c r="P3" s="1">
+        <v>81802.0</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>72256.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="D4" s="1">
-        <v>92806.0</v>
+        <v>30354.0</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="G4" s="1">
-        <v>389.0</v>
+        <v>235.0</v>
       </c>
       <c r="H4" s="1">
-        <v>1892.0</v>
+        <v>1467.0</v>
       </c>
       <c r="I4" s="1">
-        <v>846.0</v>
+        <v>976.0</v>
       </c>
       <c r="J4" s="1">
-        <v>349007.0</v>
+        <v>465230.0</v>
       </c>
       <c r="K4" s="1">
-        <v>3.1</v>
+        <v>4.2</v>
       </c>
       <c r="L4" s="1">
-        <v>34.0</v>
+        <v>33.5</v>
       </c>
       <c r="M4" s="1">
-        <v>102.5</v>
+        <v>98.8</v>
       </c>
       <c r="N4" s="1">
-        <v>97.4</v>
+        <v>103.6</v>
       </c>
       <c r="O4" s="1">
-        <v>118.0</v>
+        <v>122.7</v>
+      </c>
+      <c r="P4" s="1">
+        <v>75402.0</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>66538.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D5" s="1">
-        <v>30354.0</v>
+        <v>32952.0</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="G5" s="1">
-        <v>235.0</v>
+        <v>143.0</v>
       </c>
       <c r="H5" s="1">
-        <v>1467.0</v>
+        <v>821.0</v>
       </c>
       <c r="I5" s="1">
-        <v>976.0</v>
+        <v>829.0</v>
       </c>
       <c r="J5" s="1">
-        <v>465230.0</v>
+        <v>36380.0</v>
       </c>
       <c r="K5" s="1">
-        <v>4.2</v>
+        <v>3.5</v>
       </c>
       <c r="L5" s="1">
-        <v>33.5</v>
+        <v>49.6</v>
       </c>
       <c r="M5" s="1">
-        <v>98.8</v>
+        <v>103.3</v>
       </c>
       <c r="N5" s="1">
-        <v>103.6</v>
+        <v>97.6</v>
       </c>
       <c r="O5" s="1">
-        <v>122.7</v>
+        <v>86.4</v>
+      </c>
+      <c r="P5" s="1">
+        <v>69102.0</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>61003.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D6" s="1">
-        <v>97701.0</v>
+        <v>75074.0</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="G6" s="1">
-        <v>274.0</v>
+        <v>152.0</v>
       </c>
       <c r="H6" s="1">
-        <v>0.0</v>
+        <v>1355.0</v>
       </c>
       <c r="I6" s="1">
-        <v>0.0</v>
+        <v>935.0</v>
       </c>
       <c r="J6" s="1">
-        <v>87167.0</v>
+        <v>281566.0</v>
       </c>
       <c r="K6" s="1">
-        <v>3.6</v>
+        <v>3.2</v>
       </c>
       <c r="L6" s="1">
-        <v>38.2</v>
+        <v>38.8</v>
       </c>
       <c r="M6" s="1">
-        <v>102.2</v>
+        <v>103.0</v>
       </c>
       <c r="N6" s="1">
-        <v>83.6</v>
+        <v>100.4</v>
       </c>
       <c r="O6" s="1">
-        <v>82.6</v>
+        <v>88.0</v>
+      </c>
+      <c r="P6" s="1">
+        <v>75102.0</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>66329.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>17</v>
+        <v>44</v>
       </c>
       <c r="D7" s="1">
-        <v>94510.0</v>
+        <v>83442.0</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="G7" s="1">
-        <v>351.0</v>
+        <v>194.0</v>
       </c>
       <c r="H7" s="1">
-        <v>1991.0</v>
+        <v>775.0</v>
       </c>
       <c r="I7" s="1">
-        <v>768.0</v>
+        <v>0.0</v>
       </c>
       <c r="J7" s="1">
-        <v>28011.0</v>
+        <v>4018.0</v>
       </c>
       <c r="K7" s="1">
-        <v>3.0</v>
+        <v>2.2</v>
       </c>
       <c r="L7" s="1">
-        <v>44.9</v>
+        <v>26.6</v>
       </c>
       <c r="M7" s="1">
-        <v>110.2</v>
+        <v>92.3</v>
       </c>
       <c r="N7" s="1">
-        <v>106.0</v>
+        <v>93.0</v>
       </c>
       <c r="O7" s="1">
-        <v>120.7</v>
+        <v>85.8</v>
+      </c>
+      <c r="P7" s="1">
+        <v>68802.0</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>60744.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="D8" s="1">
-        <v>92822.0</v>
+        <v>84401.0</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="G8" s="1">
-        <v>389.0</v>
+        <v>184.0</v>
       </c>
       <c r="H8" s="1">
-        <v>1881.0</v>
+        <v>1055.0</v>
       </c>
       <c r="I8" s="1">
-        <v>813.0</v>
+        <v>930.0</v>
       </c>
       <c r="J8" s="1">
-        <v>41921.0</v>
+        <v>85497.0</v>
       </c>
       <c r="K8" s="1">
-        <v>2.9</v>
+        <v>3.8</v>
       </c>
       <c r="L8" s="1">
-        <v>37.9</v>
+        <v>31.0</v>
       </c>
       <c r="M8" s="1">
-        <v>103.5</v>
+        <v>92.3</v>
       </c>
       <c r="N8" s="1">
-        <v>99.8</v>
+        <v>95.7</v>
       </c>
       <c r="O8" s="1">
-        <v>125.5</v>
+        <v>86.9</v>
+      </c>
+      <c r="P8" s="1">
+        <v>70602.0</v>
+      </c>
+      <c r="Q8" s="1">
+        <v>62315.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="D9" s="1">
-        <v>11231.0</v>
+        <v>90211.0</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>18</v>
+        <v>52</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="G9" s="1">
-        <v>716.0</v>
+        <v>551.0</v>
       </c>
       <c r="H9" s="1">
-        <v>2951.0</v>
+        <v>2524.0</v>
       </c>
       <c r="I9" s="1">
-        <v>651.0</v>
+        <v>792.0</v>
       </c>
       <c r="J9" s="1">
-        <v>2635121.0</v>
+        <v>3949776.0</v>
       </c>
       <c r="K9" s="1">
-        <v>4.2</v>
+        <v>4.6</v>
       </c>
       <c r="L9" s="1">
-        <v>34.8</v>
+        <v>35.2</v>
       </c>
       <c r="M9" s="1">
-        <v>117.78</v>
+        <v>104.1</v>
       </c>
       <c r="N9" s="1">
-        <v>151.16</v>
+        <v>93.7</v>
       </c>
       <c r="O9" s="1">
-        <v>192.6</v>
+        <v>165.3</v>
+      </c>
+      <c r="P9" s="1">
+        <v>85802.0</v>
+      </c>
+      <c r="Q9" s="1">
+        <v>75721.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>17</v>
+        <v>51</v>
       </c>
       <c r="D10" s="1">
-        <v>91710.0</v>
+        <v>90266.0</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="G10" s="1">
-        <v>262.0</v>
+        <v>1222.0</v>
       </c>
       <c r="H10" s="1">
-        <v>1777.0</v>
+        <v>1300.0</v>
       </c>
       <c r="I10" s="1">
-        <v>919.0</v>
+        <v>660.0</v>
       </c>
       <c r="J10" s="1">
-        <v>85609.0</v>
+        <v>35698.0</v>
       </c>
       <c r="K10" s="1">
         <v>3.4</v>
       </c>
       <c r="L10" s="1">
-        <v>36.6</v>
+        <v>43.7</v>
       </c>
       <c r="M10" s="1">
-        <v>101.2</v>
+        <v>116.4</v>
       </c>
       <c r="N10" s="1">
-        <v>108.3</v>
+        <v>89.4</v>
       </c>
       <c r="O10" s="1">
-        <v>120.2</v>
+        <v>156.5</v>
+      </c>
+      <c r="P10" s="1">
+        <v>85202.0</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>75240.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="D11" s="1">
+        <v>90404.0</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" s="1">
-        <v>92879.0</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="F11" s="1" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="G11" s="1">
-        <v>251.0</v>
+        <v>1127.0</v>
       </c>
       <c r="H11" s="1">
-        <v>1757.0</v>
+        <v>3926.0</v>
       </c>
       <c r="I11" s="1">
-        <v>884.0</v>
+        <v>775.0</v>
       </c>
       <c r="J11" s="1">
-        <v>163585.0</v>
+        <v>92495.0</v>
       </c>
       <c r="K11" s="1">
-        <v>3.3</v>
+        <v>4.4</v>
       </c>
       <c r="L11" s="1">
-        <v>34.7</v>
+        <v>40.5</v>
       </c>
       <c r="M11" s="1">
-        <v>101.4</v>
+        <v>111.4</v>
       </c>
       <c r="N11" s="1">
-        <v>106.1</v>
+        <v>80.8</v>
       </c>
       <c r="O11" s="1">
-        <v>155.4</v>
+        <v>154.8</v>
+      </c>
+      <c r="P11" s="1">
+        <v>85602.0</v>
+      </c>
+      <c r="Q11" s="1">
+        <v>75613.0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>17</v>
+        <v>51</v>
       </c>
       <c r="D12" s="1">
-        <v>92627.0</v>
+        <v>90405.0</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>18</v>
+        <v>61</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="G12" s="1">
-        <v>511.0</v>
+        <v>1127.0</v>
       </c>
       <c r="H12" s="1">
-        <v>2137.0</v>
+        <v>3926.0</v>
       </c>
       <c r="I12" s="1">
-        <v>852.0</v>
+        <v>775.0</v>
       </c>
       <c r="J12" s="1">
-        <v>112930.0</v>
+        <v>92495.0</v>
       </c>
       <c r="K12" s="1">
-        <v>2.6</v>
+        <v>4.4</v>
       </c>
       <c r="L12" s="1">
-        <v>34.5</v>
+        <v>40.5</v>
       </c>
       <c r="M12" s="1">
-        <v>105.1</v>
+        <v>111.4</v>
       </c>
       <c r="N12" s="1">
-        <v>90.4</v>
+        <v>80.8</v>
       </c>
       <c r="O12" s="1">
-        <v>106.6</v>
+        <v>154.8</v>
+      </c>
+      <c r="P12" s="1">
+        <v>85602.0</v>
+      </c>
+      <c r="Q12" s="1">
+        <v>75613.0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>17</v>
+        <v>51</v>
       </c>
       <c r="D13" s="1">
-        <v>95014.0</v>
+        <v>90505.0</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="G13" s="1">
-        <v>1047.0</v>
+        <v>541.0</v>
       </c>
       <c r="H13" s="1">
-        <v>3492.0</v>
+        <v>2037.0</v>
       </c>
       <c r="I13" s="1">
-        <v>966.0</v>
+        <v>850.0</v>
       </c>
       <c r="J13" s="1">
-        <v>60687.0</v>
+        <v>147190.0</v>
       </c>
       <c r="K13" s="1">
-        <v>2.5</v>
+        <v>3.8</v>
       </c>
       <c r="L13" s="1">
-        <v>41.1</v>
+        <v>41.7</v>
       </c>
       <c r="M13" s="1">
-        <v>121.5</v>
+        <v>105.4</v>
       </c>
       <c r="N13" s="1">
-        <v>86.2</v>
+        <v>92.0</v>
       </c>
       <c r="O13" s="1">
-        <v>146.9</v>
+        <v>153.9</v>
+      </c>
+      <c r="P13" s="1">
+        <v>85002.0</v>
+      </c>
+      <c r="Q13" s="1">
+        <v>75001.0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>17</v>
+        <v>51</v>
       </c>
       <c r="D14" s="1">
         <v>90630.0</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="G14" s="1">
         <v>418.0</v>
@@ -1389,657 +1482,753 @@
       <c r="O14" s="1">
         <v>121.4</v>
       </c>
+      <c r="P14" s="1">
+        <v>85102.0</v>
+      </c>
+      <c r="Q14" s="1">
+        <v>75169.0</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>17</v>
+        <v>51</v>
       </c>
       <c r="D15" s="1">
-        <v>92610.0</v>
+        <v>90631.0</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="G15" s="1">
-        <v>433.0</v>
+        <v>387.0</v>
       </c>
       <c r="H15" s="1">
-        <v>2401.0</v>
+        <v>1817.0</v>
       </c>
       <c r="I15" s="1">
-        <v>948.0</v>
+        <v>824.0</v>
       </c>
       <c r="J15" s="1">
-        <v>12025.0</v>
+        <v>61965.0</v>
       </c>
       <c r="K15" s="1">
-        <v>2.7</v>
+        <v>3.1</v>
       </c>
       <c r="L15" s="1">
-        <v>37.7</v>
+        <v>34.7</v>
       </c>
       <c r="M15" s="1">
-        <v>103.9</v>
+        <v>102.4</v>
       </c>
       <c r="N15" s="1">
-        <v>101.7</v>
+        <v>97.9</v>
       </c>
       <c r="O15" s="1">
-        <v>114.5</v>
+        <v>121.1</v>
+      </c>
+      <c r="P15" s="1">
+        <v>85102.0</v>
+      </c>
+      <c r="Q15" s="1">
+        <v>75169.0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>17</v>
+        <v>51</v>
       </c>
       <c r="D16" s="1">
-        <v>92606.0</v>
+        <v>90670.0</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="G16" s="1">
-        <v>483.0</v>
+        <v>0.0</v>
       </c>
       <c r="H16" s="1">
-        <v>2468.0</v>
+        <v>1959.0</v>
       </c>
       <c r="I16" s="1">
-        <v>918.0</v>
+        <v>832.0</v>
       </c>
       <c r="J16" s="1">
-        <v>256877.0</v>
+        <v>17669.0</v>
       </c>
       <c r="K16" s="1">
-        <v>2.8</v>
+        <v>4.6</v>
       </c>
       <c r="L16" s="1">
-        <v>34.4</v>
+        <v>36.4</v>
       </c>
       <c r="M16" s="1">
-        <v>105.6</v>
+        <v>101.2</v>
       </c>
       <c r="N16" s="1">
-        <v>98.3</v>
+        <v>100.2</v>
       </c>
       <c r="O16" s="1">
-        <v>111.0</v>
+        <v>158.3</v>
+      </c>
+      <c r="P16" s="1">
+        <v>85002.0</v>
+      </c>
+      <c r="Q16" s="1">
+        <v>75045.0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>17</v>
+        <v>51</v>
       </c>
       <c r="D17" s="1">
-        <v>92618.0</v>
+        <v>90670.0</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="G17" s="1">
-        <v>483.0</v>
+        <v>0.0</v>
       </c>
       <c r="H17" s="1">
-        <v>2468.0</v>
+        <v>1959.0</v>
       </c>
       <c r="I17" s="1">
-        <v>918.0</v>
+        <v>832.0</v>
       </c>
       <c r="J17" s="1">
-        <v>256877.0</v>
+        <v>17669.0</v>
       </c>
       <c r="K17" s="1">
-        <v>2.8</v>
+        <v>4.6</v>
       </c>
       <c r="L17" s="1">
-        <v>34.4</v>
+        <v>36.4</v>
       </c>
       <c r="M17" s="1">
-        <v>105.6</v>
+        <v>101.2</v>
       </c>
       <c r="N17" s="1">
-        <v>98.3</v>
+        <v>100.2</v>
       </c>
       <c r="O17" s="1">
-        <v>111.0</v>
+        <v>158.3</v>
+      </c>
+      <c r="P17" s="1">
+        <v>85002.0</v>
+      </c>
+      <c r="Q17" s="1">
+        <v>75045.0</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="2" t="s">
-        <v>72</v>
+      <c r="A18" s="1" t="s">
+        <v>77</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>17</v>
+        <v>51</v>
       </c>
       <c r="D18" s="1">
-        <v>91935.0</v>
+        <v>91301.0</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>74</v>
+        <v>20</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="G18" s="1">
-        <v>282.0</v>
+        <v>430.0</v>
       </c>
       <c r="H18" s="1">
-        <v>0.0</v>
+        <v>2534.0</v>
       </c>
       <c r="I18" s="1">
-        <v>0.0</v>
+        <v>1027.0</v>
       </c>
       <c r="J18" s="1">
-        <v>5895.0</v>
+        <v>20736.0</v>
       </c>
       <c r="K18" s="1">
-        <v>3.3</v>
+        <v>4.2</v>
       </c>
       <c r="L18" s="1">
-        <v>48.3</v>
+        <v>44.0</v>
       </c>
       <c r="M18" s="1">
-        <v>109.9</v>
+        <v>105.3</v>
       </c>
       <c r="N18" s="1">
-        <v>106.9</v>
+        <v>97.3</v>
       </c>
       <c r="O18" s="1">
-        <v>137.4</v>
+        <v>158.5</v>
+      </c>
+      <c r="P18" s="1">
+        <v>83702.0</v>
+      </c>
+      <c r="Q18" s="1">
+        <v>73873.0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D19" s="1">
+        <v>91710.0</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D19" s="1">
-        <v>90631.0</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="F19" s="1" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="G19" s="1">
-        <v>387.0</v>
+        <v>262.0</v>
       </c>
       <c r="H19" s="1">
-        <v>1817.0</v>
+        <v>1777.0</v>
       </c>
       <c r="I19" s="1">
-        <v>824.0</v>
+        <v>919.0</v>
       </c>
       <c r="J19" s="1">
-        <v>61965.0</v>
+        <v>85609.0</v>
       </c>
       <c r="K19" s="1">
-        <v>3.1</v>
+        <v>3.4</v>
       </c>
       <c r="L19" s="1">
-        <v>34.7</v>
+        <v>36.6</v>
       </c>
       <c r="M19" s="1">
-        <v>102.4</v>
+        <v>101.2</v>
       </c>
       <c r="N19" s="1">
-        <v>97.9</v>
+        <v>108.3</v>
       </c>
       <c r="O19" s="1">
-        <v>121.1</v>
+        <v>120.2</v>
+      </c>
+      <c r="P19" s="1">
+        <v>83102.0</v>
+      </c>
+      <c r="Q19" s="1">
+        <v>73333.0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>79</v>
+        <v>83</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>84</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>17</v>
+        <v>51</v>
       </c>
       <c r="D20" s="1">
-        <v>90211.0</v>
+        <v>91762.0</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="G20" s="1">
-        <v>551.0</v>
+        <v>270.0</v>
       </c>
       <c r="H20" s="1">
-        <v>2524.0</v>
+        <v>1795.0</v>
       </c>
       <c r="I20" s="1">
-        <v>792.0</v>
+        <v>903.0</v>
       </c>
       <c r="J20" s="1">
-        <v>3949776.0</v>
+        <v>171041.0</v>
       </c>
       <c r="K20" s="1">
-        <v>4.6</v>
+        <v>3.6</v>
       </c>
       <c r="L20" s="1">
-        <v>35.2</v>
+        <v>32.0</v>
       </c>
       <c r="M20" s="1">
-        <v>104.1</v>
+        <v>100.7</v>
       </c>
       <c r="N20" s="1">
-        <v>93.7</v>
+        <v>105.2</v>
       </c>
       <c r="O20" s="1">
-        <v>165.3</v>
+        <v>115.2</v>
+      </c>
+      <c r="P20" s="1">
+        <v>81402.0</v>
+      </c>
+      <c r="Q20" s="1">
+        <v>71819.0</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="1" t="s">
-        <v>82</v>
+      <c r="A21" s="4" t="s">
+        <v>87</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>84</v>
+        <v>51</v>
       </c>
       <c r="D21" s="1">
-        <v>32952.0</v>
+        <v>91935.0</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>85</v>
+        <v>25</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="G21" s="1">
-        <v>143.0</v>
+        <v>282.0</v>
       </c>
       <c r="H21" s="1">
-        <v>821.0</v>
+        <v>0.0</v>
       </c>
       <c r="I21" s="1">
-        <v>829.0</v>
+        <v>0.0</v>
       </c>
       <c r="J21" s="1">
-        <v>36380.0</v>
+        <v>5895.0</v>
       </c>
       <c r="K21" s="1">
-        <v>3.5</v>
+        <v>3.3</v>
       </c>
       <c r="L21" s="1">
-        <v>49.6</v>
+        <v>48.3</v>
       </c>
       <c r="M21" s="1">
-        <v>103.3</v>
+        <v>109.9</v>
       </c>
       <c r="N21" s="1">
-        <v>97.6</v>
+        <v>106.9</v>
       </c>
       <c r="O21" s="1">
-        <v>86.4</v>
+        <v>137.4</v>
+      </c>
+      <c r="P21" s="1">
+        <v>81602.0</v>
+      </c>
+      <c r="Q21" s="1">
+        <v>72026.0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>17</v>
+        <v>51</v>
       </c>
       <c r="D22" s="1">
-        <v>92563.0</v>
+        <v>92071.0</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="G22" s="1">
-        <v>201.0</v>
+        <v>338.0</v>
       </c>
       <c r="H22" s="1">
-        <v>1706.0</v>
+        <v>1739.0</v>
       </c>
       <c r="I22" s="1">
-        <v>909.0</v>
+        <v>856.0</v>
       </c>
       <c r="J22" s="1">
-        <v>110043.0</v>
+        <v>57376.0</v>
       </c>
       <c r="K22" s="1">
-        <v>3.5</v>
+        <v>3.1</v>
       </c>
       <c r="L22" s="1">
-        <v>33.7</v>
+        <v>38.3</v>
       </c>
       <c r="M22" s="1">
-        <v>100.7</v>
+        <v>107.8</v>
       </c>
       <c r="N22" s="1">
-        <v>105.6</v>
+        <v>111.3</v>
       </c>
       <c r="O22" s="1">
-        <v>117.1</v>
+        <v>123.5</v>
+      </c>
+      <c r="P22" s="1">
+        <v>81802.0</v>
+      </c>
+      <c r="Q22" s="1">
+        <v>72241.0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>90</v>
+        <v>93</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>94</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>91</v>
+        <v>51</v>
       </c>
       <c r="D23" s="1">
-        <v>84401.0</v>
+        <v>92563.0</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="G23" s="1">
-        <v>184.0</v>
+        <v>201.0</v>
       </c>
       <c r="H23" s="1">
-        <v>1055.0</v>
+        <v>1706.0</v>
       </c>
       <c r="I23" s="1">
-        <v>930.0</v>
+        <v>909.0</v>
       </c>
       <c r="J23" s="1">
-        <v>85497.0</v>
+        <v>110043.0</v>
       </c>
       <c r="K23" s="1">
-        <v>3.8</v>
+        <v>3.5</v>
       </c>
       <c r="L23" s="1">
-        <v>31.0</v>
+        <v>33.7</v>
       </c>
       <c r="M23" s="1">
-        <v>92.3</v>
+        <v>100.7</v>
       </c>
       <c r="N23" s="1">
-        <v>95.7</v>
+        <v>105.6</v>
       </c>
       <c r="O23" s="1">
-        <v>86.9</v>
+        <v>117.1</v>
+      </c>
+      <c r="P23" s="1">
+        <v>83102.0</v>
+      </c>
+      <c r="Q23" s="1">
+        <v>73354.0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>17</v>
+        <v>51</v>
       </c>
       <c r="D24" s="1">
-        <v>91762.0</v>
+        <v>92606.0</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>95</v>
+        <v>20</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="G24" s="1">
-        <v>270.0</v>
+        <v>483.0</v>
       </c>
       <c r="H24" s="1">
-        <v>1795.0</v>
+        <v>2468.0</v>
       </c>
       <c r="I24" s="1">
-        <v>903.0</v>
+        <v>918.0</v>
       </c>
       <c r="J24" s="1">
-        <v>171041.0</v>
+        <v>256877.0</v>
       </c>
       <c r="K24" s="1">
-        <v>3.6</v>
+        <v>2.8</v>
       </c>
       <c r="L24" s="1">
-        <v>32.0</v>
+        <v>34.4</v>
       </c>
       <c r="M24" s="1">
-        <v>100.7</v>
+        <v>105.6</v>
       </c>
       <c r="N24" s="1">
-        <v>105.2</v>
+        <v>98.3</v>
       </c>
       <c r="O24" s="1">
-        <v>115.2</v>
+        <v>111.0</v>
+      </c>
+      <c r="P24" s="1">
+        <v>85002.0</v>
+      </c>
+      <c r="Q24" s="1">
+        <v>75001.0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>99</v>
+        <v>51</v>
       </c>
       <c r="D25" s="1">
-        <v>19112.0</v>
+        <v>92610.0</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>74</v>
+        <v>30</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="G25" s="1">
-        <v>180.0</v>
+        <v>433.0</v>
       </c>
       <c r="H25" s="1">
-        <v>1652.0</v>
+        <v>2401.0</v>
       </c>
       <c r="I25" s="1">
-        <v>805.0</v>
+        <v>948.0</v>
       </c>
       <c r="J25" s="1">
-        <v>1569657.0</v>
+        <v>12025.0</v>
       </c>
       <c r="K25" s="1">
-        <v>5.6</v>
+        <v>2.7</v>
       </c>
       <c r="L25" s="1">
-        <v>34.1</v>
+        <v>37.7</v>
       </c>
       <c r="M25" s="1">
-        <v>102.5</v>
+        <v>103.9</v>
       </c>
       <c r="N25" s="1">
-        <v>107.7</v>
+        <v>101.7</v>
       </c>
       <c r="O25" s="1">
-        <v>141.9</v>
+        <v>114.5</v>
+      </c>
+      <c r="P25" s="1">
+        <v>84902.0</v>
+      </c>
+      <c r="Q25" s="1">
+        <v>74974.0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>103</v>
+        <v>51</v>
       </c>
       <c r="D26" s="1">
-        <v>75074.0</v>
+        <v>92618.0</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>71</v>
+        <v>40</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="G26" s="1">
-        <v>152.0</v>
+        <v>483.0</v>
       </c>
       <c r="H26" s="1">
-        <v>1355.0</v>
+        <v>2468.0</v>
       </c>
       <c r="I26" s="1">
-        <v>935.0</v>
+        <v>918.0</v>
       </c>
       <c r="J26" s="1">
-        <v>281566.0</v>
+        <v>256877.0</v>
       </c>
       <c r="K26" s="1">
-        <v>3.2</v>
+        <v>2.8</v>
       </c>
       <c r="L26" s="1">
-        <v>38.8</v>
+        <v>34.4</v>
       </c>
       <c r="M26" s="1">
-        <v>103.0</v>
+        <v>105.6</v>
       </c>
       <c r="N26" s="1">
-        <v>100.4</v>
+        <v>98.3</v>
       </c>
       <c r="O26" s="1">
-        <v>88.0</v>
+        <v>111.0</v>
+      </c>
+      <c r="P26" s="1">
+        <v>85002.0</v>
+      </c>
+      <c r="Q26" s="1">
+        <v>75001.0</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="C27" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D27" s="1">
+        <v>92627.0</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F27" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D27" s="1">
-        <v>97209.0</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F27" s="1" t="s">
+      <c r="G27" s="1">
+        <v>511.0</v>
+      </c>
+      <c r="H27" s="1">
+        <v>2137.0</v>
+      </c>
+      <c r="I27" s="1">
+        <v>852.0</v>
+      </c>
+      <c r="J27" s="1">
+        <v>112930.0</v>
+      </c>
+      <c r="K27" s="1">
+        <v>2.6</v>
+      </c>
+      <c r="L27" s="1">
+        <v>34.5</v>
+      </c>
+      <c r="M27" s="1">
+        <v>105.1</v>
+      </c>
+      <c r="N27" s="1">
+        <v>90.4</v>
+      </c>
+      <c r="O27" s="1">
+        <v>106.6</v>
+      </c>
+      <c r="P27" s="1">
+        <v>85002.0</v>
+      </c>
+      <c r="Q27" s="1">
+        <v>75001.0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="G27" s="1">
-        <v>288.0</v>
-      </c>
-      <c r="H27" s="1">
-        <v>1499.0</v>
-      </c>
-      <c r="I27" s="1">
-        <v>765.0</v>
-      </c>
-      <c r="J27" s="1">
-        <v>630331.0</v>
-      </c>
-      <c r="K27" s="1">
-        <v>3.5</v>
-      </c>
-      <c r="L27" s="1">
-        <v>36.8</v>
-      </c>
-      <c r="M27" s="1">
-        <v>103.7</v>
-      </c>
-      <c r="N27" s="1">
-        <v>79.9</v>
-      </c>
-      <c r="O27" s="1">
-        <v>129.9</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="3" t="s">
+      <c r="B28" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="C28" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D28" s="1">
+        <v>92656.0</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F28" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D28" s="1">
-        <v>97224.0</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>107</v>
-      </c>
       <c r="G28" s="1">
-        <v>288.0</v>
+        <v>426.0</v>
       </c>
       <c r="H28" s="1">
-        <v>1499.0</v>
+        <v>2248.0</v>
       </c>
       <c r="I28" s="1">
-        <v>765.0</v>
+        <v>996.0</v>
       </c>
       <c r="J28" s="1">
-        <v>630331.0</v>
+        <v>50691.0</v>
       </c>
       <c r="K28" s="1">
-        <v>3.5</v>
+        <v>2.6</v>
       </c>
       <c r="L28" s="1">
-        <v>36.8</v>
+        <v>36.6</v>
       </c>
       <c r="M28" s="1">
-        <v>103.7</v>
+        <v>102.7</v>
       </c>
       <c r="N28" s="1">
-        <v>79.9</v>
+        <v>101.5</v>
       </c>
       <c r="O28" s="1">
-        <v>129.9</v>
+        <v>111.3</v>
+      </c>
+      <c r="P28" s="1">
+        <v>84802.0</v>
+      </c>
+      <c r="Q28" s="1">
+        <v>74866.0</v>
       </c>
     </row>
     <row r="29">
@@ -2050,43 +2239,49 @@
         <v>111</v>
       </c>
       <c r="C29" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D29" s="1">
+        <v>92806.0</v>
+      </c>
+      <c r="E29" s="1" t="s">
         <v>112</v>
-      </c>
-      <c r="D29" s="1">
-        <v>83442.0</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>113</v>
       </c>
       <c r="G29" s="1">
-        <v>194.0</v>
+        <v>389.0</v>
       </c>
       <c r="H29" s="1">
-        <v>775.0</v>
+        <v>1892.0</v>
       </c>
       <c r="I29" s="1">
-        <v>0.0</v>
+        <v>846.0</v>
       </c>
       <c r="J29" s="1">
-        <v>4018.0</v>
+        <v>349007.0</v>
       </c>
       <c r="K29" s="1">
-        <v>2.2</v>
+        <v>3.1</v>
       </c>
       <c r="L29" s="1">
-        <v>26.6</v>
+        <v>34.0</v>
       </c>
       <c r="M29" s="1">
-        <v>92.3</v>
+        <v>102.5</v>
       </c>
       <c r="N29" s="1">
-        <v>93.0</v>
+        <v>97.4</v>
       </c>
       <c r="O29" s="1">
-        <v>85.8</v>
+        <v>118.0</v>
+      </c>
+      <c r="P29" s="1">
+        <v>85102.0</v>
+      </c>
+      <c r="Q29" s="1">
+        <v>75169.0</v>
       </c>
     </row>
     <row r="30">
@@ -2097,43 +2292,49 @@
         <v>115</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>17</v>
+        <v>51</v>
       </c>
       <c r="D30" s="1">
-        <v>94402.0</v>
+        <v>92822.0</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>71</v>
+        <v>30</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>116</v>
       </c>
       <c r="G30" s="1">
-        <v>861.0</v>
+        <v>389.0</v>
       </c>
       <c r="H30" s="1">
-        <v>3357.0</v>
+        <v>1881.0</v>
       </c>
       <c r="I30" s="1">
-        <v>860.0</v>
+        <v>813.0</v>
       </c>
       <c r="J30" s="1">
-        <v>103500.0</v>
+        <v>41921.0</v>
       </c>
       <c r="K30" s="1">
-        <v>2.1</v>
+        <v>2.9</v>
       </c>
       <c r="L30" s="1">
-        <v>38.7</v>
+        <v>37.9</v>
       </c>
       <c r="M30" s="1">
-        <v>116.7</v>
+        <v>103.5</v>
       </c>
       <c r="N30" s="1">
-        <v>91.9</v>
+        <v>99.8</v>
       </c>
       <c r="O30" s="1">
-        <v>143.4</v>
+        <v>125.5</v>
+      </c>
+      <c r="P30" s="1">
+        <v>85102.0</v>
+      </c>
+      <c r="Q30" s="1">
+        <v>75169.0</v>
       </c>
     </row>
     <row r="31">
@@ -2144,43 +2345,49 @@
         <v>118</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>17</v>
+        <v>51</v>
       </c>
       <c r="D31" s="1">
-        <v>90670.0</v>
+        <v>92879.0</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>22</v>
+        <v>76</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>119</v>
       </c>
       <c r="G31" s="1">
-        <v>0.0</v>
+        <v>251.0</v>
       </c>
       <c r="H31" s="1">
-        <v>1959.0</v>
+        <v>1757.0</v>
       </c>
       <c r="I31" s="1">
-        <v>832.0</v>
+        <v>884.0</v>
       </c>
       <c r="J31" s="1">
-        <v>17669.0</v>
+        <v>163585.0</v>
       </c>
       <c r="K31" s="1">
-        <v>4.6</v>
+        <v>3.3</v>
       </c>
       <c r="L31" s="1">
-        <v>36.4</v>
+        <v>34.7</v>
       </c>
       <c r="M31" s="1">
-        <v>101.2</v>
+        <v>101.4</v>
       </c>
       <c r="N31" s="1">
-        <v>100.2</v>
+        <v>106.1</v>
       </c>
       <c r="O31" s="1">
-        <v>158.3</v>
+        <v>155.4</v>
+      </c>
+      <c r="P31" s="1">
+        <v>81402.0</v>
+      </c>
+      <c r="Q31" s="1">
+        <v>71819.0</v>
       </c>
     </row>
     <row r="32">
@@ -2191,204 +2398,228 @@
         <v>121</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>17</v>
+        <v>51</v>
       </c>
       <c r="D32" s="1">
-        <v>90670.0</v>
+        <v>94402.0</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="G32" s="1">
-        <v>0.0</v>
+        <v>861.0</v>
       </c>
       <c r="H32" s="1">
-        <v>1959.0</v>
+        <v>3357.0</v>
       </c>
       <c r="I32" s="1">
-        <v>832.0</v>
+        <v>860.0</v>
       </c>
       <c r="J32" s="1">
-        <v>17669.0</v>
+        <v>103500.0</v>
       </c>
       <c r="K32" s="1">
-        <v>4.6</v>
+        <v>2.1</v>
       </c>
       <c r="L32" s="1">
-        <v>36.4</v>
+        <v>38.7</v>
       </c>
       <c r="M32" s="1">
-        <v>101.2</v>
+        <v>116.7</v>
       </c>
       <c r="N32" s="1">
-        <v>100.2</v>
+        <v>91.9</v>
       </c>
       <c r="O32" s="1">
-        <v>158.3</v>
+        <v>143.4</v>
+      </c>
+      <c r="P32" s="1">
+        <v>92702.0</v>
+      </c>
+      <c r="Q32" s="1">
+        <v>81835.0</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>17</v>
+        <v>51</v>
       </c>
       <c r="D33" s="1">
-        <v>90404.0</v>
+        <v>94510.0</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="G33" s="1">
-        <v>1127.0</v>
+        <v>351.0</v>
       </c>
       <c r="H33" s="1">
-        <v>3926.0</v>
+        <v>1991.0</v>
       </c>
       <c r="I33" s="1">
-        <v>775.0</v>
+        <v>768.0</v>
       </c>
       <c r="J33" s="1">
-        <v>92495.0</v>
+        <v>28011.0</v>
       </c>
       <c r="K33" s="1">
-        <v>4.4</v>
+        <v>3.0</v>
       </c>
       <c r="L33" s="1">
-        <v>40.5</v>
+        <v>44.9</v>
       </c>
       <c r="M33" s="1">
-        <v>111.4</v>
+        <v>110.2</v>
       </c>
       <c r="N33" s="1">
-        <v>80.8</v>
+        <v>106.0</v>
       </c>
       <c r="O33" s="1">
-        <v>154.8</v>
+        <v>120.7</v>
+      </c>
+      <c r="P33" s="1">
+        <v>85502.0</v>
+      </c>
+      <c r="Q33" s="1">
+        <v>75472.0</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>17</v>
+        <v>51</v>
       </c>
       <c r="D34" s="1">
-        <v>90405.0</v>
+        <v>95014.0</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>127</v>
+        <v>30</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="G34" s="1">
-        <v>1127.0</v>
+        <v>1047.0</v>
       </c>
       <c r="H34" s="1">
-        <v>3926.0</v>
+        <v>3492.0</v>
       </c>
       <c r="I34" s="1">
-        <v>775.0</v>
+        <v>966.0</v>
       </c>
       <c r="J34" s="1">
-        <v>92495.0</v>
+        <v>60687.0</v>
       </c>
       <c r="K34" s="1">
-        <v>4.4</v>
+        <v>2.5</v>
       </c>
       <c r="L34" s="1">
-        <v>40.5</v>
+        <v>41.1</v>
       </c>
       <c r="M34" s="1">
-        <v>111.4</v>
+        <v>121.5</v>
       </c>
       <c r="N34" s="1">
-        <v>80.8</v>
+        <v>86.2</v>
       </c>
       <c r="O34" s="1">
-        <v>154.8</v>
+        <v>146.9</v>
+      </c>
+      <c r="P34" s="1">
+        <v>95602.0</v>
+      </c>
+      <c r="Q34" s="1">
+        <v>84391.0</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>17</v>
+        <v>51</v>
       </c>
       <c r="D35" s="1">
-        <v>92071.0</v>
+        <v>95066.0</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>85</v>
+        <v>48</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="G35" s="1">
-        <v>338.0</v>
+        <v>484.0</v>
       </c>
       <c r="H35" s="1">
-        <v>1739.0</v>
+        <v>0.0</v>
       </c>
       <c r="I35" s="1">
-        <v>856.0</v>
+        <v>0.0</v>
       </c>
       <c r="J35" s="1">
-        <v>57376.0</v>
+        <v>11892.0</v>
       </c>
       <c r="K35" s="1">
-        <v>3.1</v>
+        <v>4.8</v>
       </c>
       <c r="L35" s="1">
-        <v>38.3</v>
+        <v>39.7</v>
       </c>
       <c r="M35" s="1">
-        <v>107.8</v>
+        <v>112.1</v>
       </c>
       <c r="N35" s="1">
-        <v>111.3</v>
+        <v>102.9</v>
       </c>
       <c r="O35" s="1">
-        <v>123.5</v>
+        <v>117.0</v>
+      </c>
+      <c r="P35" s="1">
+        <v>84802.0</v>
+      </c>
+      <c r="Q35" s="1">
+        <v>74866.0</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>17</v>
+        <v>51</v>
       </c>
       <c r="D36" s="1">
         <v>95066.0</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G36" s="1">
         <v>484.0</v>
@@ -2416,6 +2647,12 @@
       </c>
       <c r="O36" s="1">
         <v>117.0</v>
+      </c>
+      <c r="P36" s="1">
+        <v>84802.0</v>
+      </c>
+      <c r="Q36" s="1">
+        <v>74866.0</v>
       </c>
     </row>
     <row r="37">
@@ -2426,150 +2663,172 @@
         <v>135</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="D37" s="1">
-        <v>95066.0</v>
+        <v>97209.0</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="G37" s="1">
-        <v>484.0</v>
+        <v>288.0</v>
       </c>
       <c r="H37" s="1">
-        <v>0.0</v>
+        <v>1499.0</v>
       </c>
       <c r="I37" s="1">
-        <v>0.0</v>
+        <v>765.0</v>
       </c>
       <c r="J37" s="1">
-        <v>11892.0</v>
+        <v>630331.0</v>
       </c>
       <c r="K37" s="1">
-        <v>4.8</v>
+        <v>3.5</v>
       </c>
       <c r="L37" s="1">
-        <v>39.7</v>
+        <v>36.8</v>
       </c>
       <c r="M37" s="1">
-        <v>112.1</v>
+        <v>103.7</v>
       </c>
       <c r="N37" s="1">
-        <v>102.9</v>
+        <v>79.9</v>
       </c>
       <c r="O37" s="1">
-        <v>117.0</v>
+        <v>129.9</v>
+      </c>
+      <c r="P37" s="1">
+        <v>79602.0</v>
+      </c>
+      <c r="Q37" s="1">
+        <v>70306.0</v>
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="1" t="s">
+      <c r="A38" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C38" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="D38" s="1">
+        <v>97224.0</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F38" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="C38" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D38" s="1">
-        <v>90505.0</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>138</v>
-      </c>
       <c r="G38" s="1">
-        <v>541.0</v>
+        <v>288.0</v>
       </c>
       <c r="H38" s="1">
-        <v>2037.0</v>
+        <v>1499.0</v>
       </c>
       <c r="I38" s="1">
-        <v>850.0</v>
+        <v>765.0</v>
       </c>
       <c r="J38" s="1">
-        <v>147190.0</v>
+        <v>630331.0</v>
       </c>
       <c r="K38" s="1">
-        <v>3.8</v>
+        <v>3.5</v>
       </c>
       <c r="L38" s="1">
-        <v>41.7</v>
+        <v>36.8</v>
       </c>
       <c r="M38" s="1">
-        <v>105.4</v>
+        <v>103.7</v>
       </c>
       <c r="N38" s="1">
-        <v>92.0</v>
+        <v>79.9</v>
       </c>
       <c r="O38" s="1">
-        <v>153.9</v>
+        <v>129.9</v>
+      </c>
+      <c r="P38" s="1">
+        <v>79602.0</v>
+      </c>
+      <c r="Q38" s="1">
+        <v>70306.0</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>141</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="D39" s="1">
-        <v>90266.0</v>
+        <v>97701.0</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="G39" s="1">
-        <v>1222.0</v>
+        <v>274.0</v>
       </c>
       <c r="H39" s="1">
-        <v>1300.0</v>
+        <v>0.0</v>
       </c>
       <c r="I39" s="1">
-        <v>660.0</v>
+        <v>0.0</v>
       </c>
       <c r="J39" s="1">
-        <v>35698.0</v>
+        <v>87167.0</v>
       </c>
       <c r="K39" s="1">
-        <v>3.4</v>
+        <v>3.6</v>
       </c>
       <c r="L39" s="1">
-        <v>43.7</v>
+        <v>38.2</v>
       </c>
       <c r="M39" s="1">
-        <v>116.4</v>
+        <v>102.2</v>
       </c>
       <c r="N39" s="1">
-        <v>89.4</v>
+        <v>83.6</v>
       </c>
       <c r="O39" s="1">
-        <v>156.5</v>
+        <v>82.6</v>
+      </c>
+      <c r="P39" s="1">
+        <v>73702.0</v>
+      </c>
+      <c r="Q39" s="1">
+        <v>65019.0</v>
       </c>
     </row>
     <row r="52">
-      <c r="D52" s="4" t="s">
-        <v>141</v>
+      <c r="D52" s="6" t="s">
+        <v>143</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="$A$1:$Z$39">
     <sortState ref="A1:Z39">
+      <sortCondition ref="D1:D39"/>
       <sortCondition ref="F1:F39"/>
     </sortState>
   </autoFilter>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="A18"/>
-    <hyperlink r:id="rId2" ref="A28"/>
+    <hyperlink r:id="rId1" ref="A21"/>
+    <hyperlink r:id="rId2" ref="A38"/>
     <hyperlink r:id="rId3" ref="D52"/>
   </hyperlinks>
   <drawing r:id="rId4"/>

</xml_diff>